<commit_message>
finished peak picks, about to do final calculations
</commit_message>
<xml_diff>
--- a/N_xi Fits/Figures/N_xi Fitted Parameters (rho=0.7).xlsx
+++ b/N_xi Fits/Figures/N_xi Fitted Parameters (rho=0.7).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -491,32 +491,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1232.77587890625</v>
+        <v>4355.316285329744</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02369471006966117</v>
+        <v>0.0193185465325742</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0002845861573893906</v>
+        <v>0.001953093224947348</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8461366212105671</v>
+        <v>0.1395229641860062</v>
       </c>
       <c r="H2" t="n">
-        <v>0.008041906361808482</v>
+        <v>0.004610317849595487</v>
       </c>
       <c r="I2" t="n">
-        <v>8.460775595800112e-05</v>
+        <v>1.778342606275174e-05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -524,32 +524,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2164.0869140625</v>
+        <v>7450.874831763122</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01690014782560962</v>
+        <v>0.01318072612304128</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001818803637416336</v>
+        <v>0.000365849681011876</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8168257064733345</v>
+        <v>0.3025351376448336</v>
       </c>
       <c r="H3" t="n">
-        <v>0.006642855859159765</v>
+        <v>0.005136858254094076</v>
       </c>
       <c r="I3" t="n">
-        <v>5.753243681173123e-05</v>
+        <v>1.812645363354558e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -557,32 +557,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3714.4775390625</v>
+        <v>8457.604306864065</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01095795598542008</v>
+        <v>0.009881874496958173</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0001427613453175447</v>
+        <v>0.0007891930860704901</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9144341617597561</v>
+        <v>0.4217412377205599</v>
       </c>
       <c r="H4" t="n">
-        <v>0.009518647339887651</v>
+        <v>0.02435912147581138</v>
       </c>
       <c r="I4" t="n">
-        <v>7.240582795943693e-05</v>
+        <v>0.0005634149322016302</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -590,26 +590,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4500.439453125</v>
+        <v>9039.030955585464</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01073577425162403</v>
+        <v>0.009160135482986668</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0001550291212553833</v>
+        <v>0.0003745730122605985</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5140809771811112</v>
+        <v>0.5161655294932277</v>
       </c>
       <c r="H5" t="n">
-        <v>0.006372120076804265</v>
+        <v>0.01582913101490795</v>
       </c>
       <c r="I5" t="n">
-        <v>9.11442629781985e-06</v>
+        <v>0.0002175416958362685</v>
       </c>
     </row>
     <row r="6">
@@ -619,30 +619,30 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4355.316285329744</v>
+        <v>6896.36608344549</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01668302507597138</v>
+        <v>0.02224225204176123</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00178558457375996</v>
+        <v>0.0008391192869601676</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1442421300639544</v>
+        <v>0.1702259955295795</v>
       </c>
       <c r="H6" t="n">
-        <v>0.004968714203042109</v>
+        <v>0.002586638875748163</v>
       </c>
       <c r="I6" t="n">
-        <v>1.383052966919092e-05</v>
+        <v>6.829394177994702e-06</v>
       </c>
     </row>
     <row r="7">
@@ -652,30 +652,30 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7450.874831763122</v>
+        <v>7940.780619111709</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0128653765363228</v>
+        <v>0.01663964670364464</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000406118551458666</v>
+        <v>0.0002130071679219476</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3057201368360177</v>
+        <v>0.5100270109795788</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005593981817637108</v>
+        <v>0.004735669300199534</v>
       </c>
       <c r="I7" t="n">
-        <v>1.741412141094241e-05</v>
+        <v>2.561962818258514e-05</v>
       </c>
     </row>
     <row r="8">
@@ -685,30 +685,30 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8457.604306864065</v>
+        <v>8861.372812920592</v>
       </c>
       <c r="E8" t="n">
-        <v>0.008878593860629305</v>
+        <v>0.01340545014843422</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0006740014911800973</v>
+        <v>0.0004453470815795779</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4453019184510856</v>
+        <v>0.409474197951006</v>
       </c>
       <c r="H8" t="n">
-        <v>0.02434217434166221</v>
+        <v>0.009376623745287997</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0004372916797051629</v>
+        <v>8.362671042924979e-05</v>
       </c>
     </row>
     <row r="9">
@@ -718,162 +718,162 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>9039.030955585464</v>
+        <v>9270.524899057873</v>
       </c>
       <c r="E9" t="n">
-        <v>0.008440743976044477</v>
+        <v>0.005969433836888237</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0002463414597824362</v>
+        <v>0.0004893413899219859</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5383654301469857</v>
+        <v>0.24268244005037</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01136229301178075</v>
+        <v>0.01386187683863055</v>
       </c>
       <c r="I9" t="n">
-        <v>8.513119431760379e-05</v>
+        <v>3.973983113378897e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>963.61083984375</v>
+        <v>5625.54931640625</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02545756072541457</v>
+        <v>0.02568278068954721</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0007129638304308419</v>
+        <v>0.001421340953411223</v>
       </c>
       <c r="G10" t="n">
-        <v>0.507131127463651</v>
+        <v>0.3142039078416817</v>
       </c>
       <c r="H10" t="n">
-        <v>0.009732346801476622</v>
+        <v>0.01119145378037536</v>
       </c>
       <c r="I10" t="n">
-        <v>7.526560440424825e-05</v>
+        <v>0.0002285141756953128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3030.79833984375</v>
+        <v>8096.484375</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04262091589742936</v>
+        <v>0.01344428179306977</v>
       </c>
       <c r="F11" t="n">
-        <v>0.006663265935112016</v>
+        <v>0.0002101982536333677</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3481215743158039</v>
+        <v>0.3399167085646607</v>
       </c>
       <c r="H11" t="n">
-        <v>0.02286836597409013</v>
+        <v>0.003403816468656327</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00248991890359387</v>
+        <v>9.386234963598003e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3159.99755859375</v>
+        <v>8484.08203125</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01566669608866246</v>
+        <v>0.02628248889502833</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0003252664807714755</v>
+        <v>0.001012026309988478</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7773390610498654</v>
+        <v>0.4906584519814488</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01182760505575117</v>
+        <v>0.01287140840858256</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0002163642738901038</v>
+        <v>0.0005887824444192463</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3956.72607421875</v>
+        <v>9862.20703125</v>
       </c>
       <c r="E13" t="n">
-        <v>0.009603954221091575</v>
+        <v>0.01237531692534578</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0001781612962160554</v>
+        <v>0.0003321444590674683</v>
       </c>
       <c r="G13" t="n">
-        <v>0.671072018431777</v>
+        <v>0.2720360671717537</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01008066997109111</v>
+        <v>0.004003353571977314</v>
       </c>
       <c r="I13" t="n">
-        <v>5.774231233055401e-05</v>
+        <v>1.424677507042769e-05</v>
       </c>
     </row>
     <row r="14">
@@ -883,30 +883,30 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6896.36608344549</v>
+        <v>4931.103515625</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01995499973570294</v>
+        <v>0.02457450190158904</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0006371583372481096</v>
+        <v>0.0004481135553120651</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1754456096117033</v>
+        <v>0.1527614747598163</v>
       </c>
       <c r="H14" t="n">
-        <v>0.002035247853796832</v>
+        <v>0.000993359328471914</v>
       </c>
       <c r="I14" t="n">
-        <v>2.431029340964286e-06</v>
+        <v>5.520038186021344e-07</v>
       </c>
     </row>
     <row r="15">
@@ -916,30 +916,30 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7940.780619111709</v>
+        <v>6992.90771484375</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01652578319385785</v>
+        <v>0.01788148886382257</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0002592650727460743</v>
+        <v>0.0001869509085994334</v>
       </c>
       <c r="G15" t="n">
-        <v>0.5117977140336143</v>
+        <v>0.7208777322592888</v>
       </c>
       <c r="H15" t="n">
-        <v>0.005471794925111803</v>
+        <v>0.005639806619463781</v>
       </c>
       <c r="I15" t="n">
-        <v>2.901230894465395e-05</v>
+        <v>4.659701987717247e-05</v>
       </c>
     </row>
     <row r="16">
@@ -949,30 +949,30 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8861.372812920592</v>
+        <v>7450.48828125</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01306618572993858</v>
+        <v>0.01531492026405993</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0004537704225943658</v>
+        <v>0.001373462313850816</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4145833510509899</v>
+        <v>0.1816543337830513</v>
       </c>
       <c r="H16" t="n">
-        <v>0.009648702389644262</v>
+        <v>0.007618799815753608</v>
       </c>
       <c r="I16" t="n">
-        <v>7.777215302529887e-05</v>
+        <v>5.993446292606512e-05</v>
       </c>
     </row>
     <row r="17">
@@ -982,690 +982,162 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>9270.524899057873</v>
+        <v>9878.35693359375</v>
       </c>
       <c r="E17" t="n">
-        <v>0.005098797994117952</v>
+        <v>0.1532683010408443</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0002208066195182383</v>
+        <v>0.07166011668745483</v>
       </c>
       <c r="G17" t="n">
-        <v>0.264026083369219</v>
+        <v>0.1386773889562471</v>
       </c>
       <c r="H17" t="n">
-        <v>0.00786577853163881</v>
+        <v>0.01092199169031832</v>
       </c>
       <c r="I17" t="n">
-        <v>6.03065524723741e-06</v>
+        <v>0.00100509079985503</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1808.7890625</v>
+        <v>904.39453125</v>
       </c>
       <c r="E18" t="n">
-        <v>0.09395991591137184</v>
+        <v>0.4842793268339153</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02984088559369603</v>
+        <v>0.001908598393472982</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2780784864922059</v>
+        <v>0.9021401228351151</v>
       </c>
       <c r="H18" t="n">
-        <v>0.02055292878212153</v>
+        <v>0.002661429270373424</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002814055086601161</v>
+        <v>0.0004065235854732301</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2169.47021484375</v>
+        <v>1518.0908203125</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01702419354796653</v>
+        <v>0.3832107514686146</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0003720878962279285</v>
+        <v>0.001077367409704351</v>
       </c>
       <c r="G19" t="n">
-        <v>1.021688528901814</v>
+        <v>1.039696095494624</v>
       </c>
       <c r="H19" t="n">
-        <v>0.01587338895208751</v>
+        <v>0.002190705121528471</v>
       </c>
       <c r="I19" t="n">
-        <v>0.000437028126507446</v>
+        <v>0.0001954976909446787</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3111.5478515625</v>
+        <v>2040.27099609375</v>
       </c>
       <c r="E20" t="n">
-        <v>0.009504209469428277</v>
+        <v>0.2692127130766679</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0001746062288646727</v>
+        <v>0.001237618494201748</v>
       </c>
       <c r="G20" t="n">
-        <v>0.8793031453282341</v>
+        <v>0.9620902186494883</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01486425044681404</v>
+        <v>0.003174786133403373</v>
       </c>
       <c r="I20" t="n">
-        <v>8.445984264165524e-05</v>
+        <v>0.0004291937523511609</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3477.6123046875</v>
+        <v>2697.03369140625</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01094723012484922</v>
+        <v>0.08326029484050256</v>
       </c>
       <c r="F21" t="n">
-        <v>0.000205359195661872</v>
+        <v>0.001109814641365191</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8206997967695988</v>
+        <v>0.4409908213593057</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01407596561638522</v>
+        <v>0.003671008443831235</v>
       </c>
       <c r="I21" t="n">
-        <v>6.283518743798449e-05</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>TAG6rearSOAEwf1.mat</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>5625.54931640625</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.01900785330173502</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.0004625698288854586</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.3624474496523025</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.005487717647863577</v>
-      </c>
-      <c r="I22" t="n">
-        <v>2.182543758349044e-05</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>TAG6rearSOAEwf1.mat</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>8096.484375</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.01321688259135365</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.0002082230006732784</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.342523361251309</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.003294343549051941</v>
-      </c>
-      <c r="I23" t="n">
-        <v>7.474952133478373e-06</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>TAG6rearSOAEwf1.mat</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>8484.08203125</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.02170707159635535</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.0004739967257639818</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.5338984949776205</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.007543446134174521</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.0001340456844572405</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>2</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>TAG6rearSOAEwf1.mat</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>9862.20703125</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.01238732169044218</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.0004327665110941091</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.2719524639682749</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.004756343091704879</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1.667667340861007e-05</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Anole</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>1803.40576171875</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0162244917506017</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.0002934703898975568</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.6332416811819169</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.008053179958807789</v>
-      </c>
-      <c r="I26" t="n">
-        <v>9.967928833420409e-05</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Anole</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>2137.17041015625</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.01008053669852845</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.0003410137885113808</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.4257857902718375</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.01034700350866422</v>
-      </c>
-      <c r="I27" t="n">
-        <v>5.046965189196347e-05</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Anole</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>3</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>2406.33544921875</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.009291863624296858</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.0004061243225305231</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.3235388380522209</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.01073642861953254</v>
-      </c>
-      <c r="I28" t="n">
-        <v>1.873718062916182e-05</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Anole</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>2777.783203125</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.009104721604838883</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.0003141571035650699</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.3304274061944039</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.007963257472636348</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1.921384668044185e-05</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>TAG9rearSOAEwf2.mat</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>4931.103515625</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.02554945086205718</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.0002878809250188784</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.1512395469372439</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.0005272524944185233</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1.10475432716849e-07</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>3</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>TAG9rearSOAEwf2.mat</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>6992.90771484375</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.01783908280497109</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.0002088436889747073</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.7217622102658805</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.006119929533740822</v>
-      </c>
-      <c r="I31" t="n">
-        <v>5.084646980469873e-05</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>TAG9rearSOAEwf2.mat</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>7450.48828125</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.01200775491462731</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.0009137669605578868</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.1965258377534159</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.006852512545787379</v>
-      </c>
-      <c r="I32" t="n">
-        <v>2.61350286580711e-05</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Owl</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>TAG9rearSOAEwf2.mat</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>9878.35693359375</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.007925407756881388</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.0003166523849149099</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.3259428593438031</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.008603468364547737</v>
-      </c>
-      <c r="I33" t="n">
-        <v>3.303956231205425e-05</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>3</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>TH13RearwaveformSOAE.mat</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>904.39453125</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.4774975069364109</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.002015795101683199</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.9085519680495239</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0.002794537494154089</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0.0004171033007098175</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>TH13RearwaveformSOAE.mat</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>1518.0908203125</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.3859203547576784</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.001157363097161739</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1.036016231513753</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.002254808448945659</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0.0001985759229047315</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>3</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>TH13RearwaveformSOAE.mat</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>2040.27099609375</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.2641542516650234</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.001184943279000272</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.9704259037510385</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.003049452986642946</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0.0003721331200152095</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>TH13RearwaveformSOAE.mat</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>2697.03369140625</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.08660014817551449</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.001596791648516694</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.4333261943010564</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.0043389060933921</v>
-      </c>
-      <c r="I37" t="n">
-        <v>4.104752251226488e-05</v>
+        <v>3.926403002096487e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before changing decay star method
</commit_message>
<xml_diff>
--- a/N_xi Fits/Figures/N_xi Fitted Parameters (rho=0.7).xlsx
+++ b/N_xi Fits/Figures/N_xi Fitted Parameters (rho=0.7).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -491,32 +491,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4355.316285329744</v>
+        <v>1232.77587890625</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0193185465325742</v>
+        <v>0.02371772119569222</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001953093224947348</v>
+        <v>0.0002456927251929869</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1395229641860062</v>
+        <v>0.8456466698789188</v>
       </c>
       <c r="H2" t="n">
-        <v>0.004610317849595487</v>
+        <v>0.007192490463702059</v>
       </c>
       <c r="I2" t="n">
-        <v>1.778342606275174e-05</v>
+        <v>7.466274220765773e-05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -524,32 +524,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7450.874831763122</v>
+        <v>2164.0869140625</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01318072612304128</v>
+        <v>0.01703730153458072</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000365849681011876</v>
+        <v>0.0001713159273487219</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3025351376448336</v>
+        <v>0.8132466454579124</v>
       </c>
       <c r="H3" t="n">
-        <v>0.005136858254094076</v>
+        <v>0.006389513498193741</v>
       </c>
       <c r="I3" t="n">
-        <v>1.812645363354558e-05</v>
+        <v>5.848417043130242e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -557,32 +557,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8457.604306864065</v>
+        <v>3714.4775390625</v>
       </c>
       <c r="E4" t="n">
-        <v>0.009881874496958173</v>
+        <v>0.01097642001908386</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0007891930860704901</v>
+        <v>0.0001307157651274837</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4217412377205599</v>
+        <v>0.913543811082511</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02435912147581138</v>
+        <v>0.008881928360398802</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0005634149322016302</v>
+        <v>6.687510118211793e-05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -590,32 +590,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9039.030955585464</v>
+        <v>4500.439453125</v>
       </c>
       <c r="E5" t="n">
-        <v>0.009160135482986668</v>
+        <v>0.01092790068540736</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0003745730122605985</v>
+        <v>0.0001669908397537451</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5161655294932277</v>
+        <v>0.5077504428804336</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01582913101490795</v>
+        <v>0.006860502286096762</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0002175416958362685</v>
+        <v>1.298890785275758e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -623,32 +623,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6896.36608344549</v>
+        <v>963.61083984375</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02224225204176123</v>
+        <v>0.02452788700632904</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0008391192869601676</v>
+        <v>0.0006789174475207971</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1702259955295795</v>
+        <v>0.5174998139483792</v>
       </c>
       <c r="H6" t="n">
-        <v>0.002586638875748163</v>
+        <v>0.0105519055586837</v>
       </c>
       <c r="I6" t="n">
-        <v>6.829394177994702e-06</v>
+        <v>9.684336360622086e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -656,32 +656,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7940.780619111709</v>
+        <v>3030.79833984375</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01663964670364464</v>
+        <v>0.03900783315061987</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0002130071679219476</v>
+        <v>0.0005269959073626083</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5100270109795788</v>
+        <v>0.3776349227635817</v>
       </c>
       <c r="H7" t="n">
-        <v>0.004735669300199534</v>
+        <v>0.003448648654001608</v>
       </c>
       <c r="I7" t="n">
-        <v>2.561962818258514e-05</v>
+        <v>1.429012607810583e-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -689,32 +689,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8861.372812920592</v>
+        <v>3159.99755859375</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01340545014843422</v>
+        <v>0.01603634877364303</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0004453470815795779</v>
+        <v>0.0003389837853600677</v>
       </c>
       <c r="G8" t="n">
-        <v>0.409474197951006</v>
+        <v>0.768175259071163</v>
       </c>
       <c r="H8" t="n">
-        <v>0.009376623745287997</v>
+        <v>0.01221283482847962</v>
       </c>
       <c r="I8" t="n">
-        <v>8.362671042924979e-05</v>
+        <v>0.0002548285078866734</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -722,32 +722,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>9270.524899057873</v>
+        <v>3956.72607421875</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005969433836888237</v>
+        <v>0.009917970099062774</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0004893413899219859</v>
+        <v>0.0002274025006255379</v>
       </c>
       <c r="G9" t="n">
-        <v>0.24268244005037</v>
+        <v>0.6581630051280913</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01386187683863055</v>
+        <v>0.01252713218740946</v>
       </c>
       <c r="I9" t="n">
-        <v>3.973983113378897e-05</v>
+        <v>0.000105036125935039</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -755,32 +755,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5625.54931640625</v>
+        <v>1808.7890625</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02568278068954721</v>
+        <v>0.03376276429862794</v>
       </c>
       <c r="F10" t="n">
-        <v>0.001421340953411223</v>
+        <v>0.0009117055675593588</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3142039078416817</v>
+        <v>0.4783748169228471</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01119145378037536</v>
+        <v>0.01050058564977139</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0002285141756953128</v>
+        <v>8.497494191901548e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -788,32 +788,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>8096.484375</v>
+        <v>2169.47021484375</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01344428179306977</v>
+        <v>0.01679552502362724</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0002101982536333677</v>
+        <v>0.000352611337226295</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3399167085646607</v>
+        <v>1.028353287840922</v>
       </c>
       <c r="H11" t="n">
-        <v>0.003403816468656327</v>
+        <v>0.01590815126020107</v>
       </c>
       <c r="I11" t="n">
-        <v>9.386234963598003e-06</v>
+        <v>0.0004568235018808497</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -821,32 +821,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>8484.08203125</v>
+        <v>3111.5478515625</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02628248889502833</v>
+        <v>0.01041321939968769</v>
       </c>
       <c r="F12" t="n">
-        <v>0.001012026309988478</v>
+        <v>0.0003715413575148304</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4906584519814488</v>
+        <v>0.8232490140236187</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01287140840858256</v>
+        <v>0.02739466501301934</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0005887824444192463</v>
+        <v>0.0004201820851399775</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -854,32 +854,32 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>9862.20703125</v>
+        <v>3477.6123046875</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01237531692534578</v>
+        <v>0.01097268786181369</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0003321444590674683</v>
+        <v>0.0001711324508200723</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2720360671717537</v>
+        <v>0.8192833706324124</v>
       </c>
       <c r="H13" t="n">
-        <v>0.004003353571977314</v>
+        <v>0.0121352699888301</v>
       </c>
       <c r="I13" t="n">
-        <v>1.424677507042769e-05</v>
+        <v>5.449628462356065e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -887,32 +887,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4931.103515625</v>
+        <v>1803.40576171875</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02457450190158904</v>
+        <v>0.01667571165285841</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0004481135553120651</v>
+        <v>0.0003246718843450537</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1527614747598163</v>
+        <v>0.6248287815927495</v>
       </c>
       <c r="H14" t="n">
-        <v>0.000993359328471914</v>
+        <v>0.008828612048560633</v>
       </c>
       <c r="I14" t="n">
-        <v>5.520038186021344e-07</v>
+        <v>0.0001347397148517859</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -920,32 +920,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>6992.90771484375</v>
+        <v>2137.17041015625</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01788148886382257</v>
+        <v>0.03209558801781425</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0001869509085994334</v>
+        <v>0.004385587038475059</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7208777322592888</v>
+        <v>0.2465319235049012</v>
       </c>
       <c r="H15" t="n">
-        <v>0.005639806619463781</v>
+        <v>0.01888068543355091</v>
       </c>
       <c r="I15" t="n">
-        <v>4.659701987717247e-05</v>
+        <v>0.00132069196281973</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -953,32 +953,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7450.48828125</v>
+        <v>2406.33544921875</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01531492026405993</v>
+        <v>0.01397454080576071</v>
       </c>
       <c r="F16" t="n">
-        <v>0.001373462313850816</v>
+        <v>0.001421054477310901</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1816543337830513</v>
+        <v>0.255853371442979</v>
       </c>
       <c r="H16" t="n">
-        <v>0.007618799815753608</v>
+        <v>0.01788279795692268</v>
       </c>
       <c r="I16" t="n">
-        <v>5.993446292606512e-05</v>
+        <v>0.0001918639613534989</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -986,157 +986,949 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>9878.35693359375</v>
+        <v>2777.783203125</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1532683010408443</v>
+        <v>0.009266631074794815</v>
       </c>
       <c r="F17" t="n">
-        <v>0.07166011668745483</v>
+        <v>0.0003053662627505908</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1386773889562471</v>
+        <v>0.3273128428440964</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01092199169031832</v>
+        <v>0.00771681905474595</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00100509079985503</v>
+        <v>2.083696922508052e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>904.39453125</v>
+        <v>4355.316285329744</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4842793268339153</v>
+        <v>0.0193185465325742</v>
       </c>
       <c r="F18" t="n">
-        <v>0.001908598393472982</v>
+        <v>0.001953093224947348</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9021401228351151</v>
+        <v>0.1395229641860062</v>
       </c>
       <c r="H18" t="n">
-        <v>0.002661429270373424</v>
+        <v>0.004610317849595487</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0004065235854732301</v>
+        <v>1.778342606275174e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1518.0908203125</v>
+        <v>7450.874831763122</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3832107514686146</v>
+        <v>0.01318072612304128</v>
       </c>
       <c r="F19" t="n">
-        <v>0.001077367409704351</v>
+        <v>0.000365849681011876</v>
       </c>
       <c r="G19" t="n">
-        <v>1.039696095494624</v>
+        <v>0.3025351376448336</v>
       </c>
       <c r="H19" t="n">
-        <v>0.002190705121528471</v>
+        <v>0.005136858254094076</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0001954976909446787</v>
+        <v>1.812645363354558e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2040.27099609375</v>
+        <v>8457.604306864065</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2692127130766679</v>
+        <v>0.009881874496958173</v>
       </c>
       <c r="F20" t="n">
-        <v>0.001237618494201748</v>
+        <v>0.0007891930860704901</v>
       </c>
       <c r="G20" t="n">
-        <v>0.9620902186494883</v>
+        <v>0.4217412377205599</v>
       </c>
       <c r="H20" t="n">
-        <v>0.003174786133403373</v>
+        <v>0.02435912147581138</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0004291937523511609</v>
+        <v>0.0005634149322016302</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Owl2R1.mat</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>9039.030955585464</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.009160135482986668</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0003745730122605985</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.5161655294932277</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.01582913101490795</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.0002175416958362685</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Owl7L1.mat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>6896.36608344549</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.02224225204176123</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0008391192869601676</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1702259955295795</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.002586638875748163</v>
+      </c>
+      <c r="I22" t="n">
+        <v>6.829394177994702e-06</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Owl7L1.mat</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>7940.780619111709</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.01663964670364464</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0002130071679219476</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.5100270109795788</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.004735669300199534</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2.561962818258514e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Owl7L1.mat</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>8861.372812920592</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.01340545014843422</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0004453470815795779</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.409474197951006</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.009376623745287997</v>
+      </c>
+      <c r="I24" t="n">
+        <v>8.362671042924979e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Owl7L1.mat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>9270.524899057873</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.005969433836888237</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0004893413899219859</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.24268244005037</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.01386187683863055</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3.973983113378897e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>TAG6rearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>5625.54931640625</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.02568278068954721</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.001421340953411223</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.3142039078416817</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.01119145378037536</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0002285141756953128</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>TAG6rearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>8096.484375</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.01344428179306977</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0002101982536333677</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.3399167085646607</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.003403816468656327</v>
+      </c>
+      <c r="I27" t="n">
+        <v>9.386234963598003e-06</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>TAG6rearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>8484.08203125</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.02628248889502833</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.001012026309988478</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.4906584519814488</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.01287140840858256</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0005887824444192463</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>TAG6rearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>9862.20703125</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.01237531692534578</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0003321444590674683</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.2720360671717537</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.004003353571977314</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.424677507042769e-05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>TAG9rearSOAEwf2.mat</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4931.103515625</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.02457450190158904</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.0004481135553120651</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1527614747598163</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.000993359328471914</v>
+      </c>
+      <c r="I30" t="n">
+        <v>5.520038186021344e-07</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>TAG9rearSOAEwf2.mat</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>6992.90771484375</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.01788148886382257</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0001869509085994334</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.7208777322592888</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.005639806619463781</v>
+      </c>
+      <c r="I31" t="n">
+        <v>4.659701987717247e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>TAG9rearSOAEwf2.mat</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>7450.48828125</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.01531492026405993</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.001373462313850816</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.1816543337830513</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.007618799815753608</v>
+      </c>
+      <c r="I32" t="n">
+        <v>5.993446292606512e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Owl</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TAG9rearSOAEwf2.mat</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>9878.35693359375</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1532683010408443</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.07166011668745483</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.1386773889562471</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.01092199169031832</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.00100509079985503</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>Human</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ALrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2664.73388671875</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.3198975460354587</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.1132362825543657</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.1657674705651171</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.007175489272441667</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.0007772644697649273</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ALrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2944.66552734375</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.1198079706415459</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.001171970465477583</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.8319410731485042</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.005789918364811536</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.0002648060372555972</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ALrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>3219.2138671875</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4836265480305565</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.004060257613187699</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.002963786288552</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.006012176359789696</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.003646294498494776</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ALrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>3865.2099609375</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.1577177893969854</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.001097030920134901</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.8454946615161817</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.004023596636132857</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.0002362468726994391</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>LSrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>732.12890625</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.5075030815554784</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.001438096912462241</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1.163054190680906</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.002587913560844039</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.0002470706988969692</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LSrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>985.14404296875</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.058192370706142</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.002750720205159487</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.9676972740012839</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.001219814487927853</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.0001003292345755535</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>LSrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1636.5234375</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.127318273592988</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.003105581816240508</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.6806637243489133</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.01246724644496831</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.0004784872595877058</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>LSrearSOAEwf1.mat</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2228.6865234375</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.373400865984132</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.001459815331236329</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.035730945915035</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.002941818263382401</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.000368024792670114</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>3</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D42" t="n">
+        <v>904.39453125</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.4842793268339153</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.001908598393472982</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.9021401228351151</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.002661429270373424</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.0004065235854732301</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>TH13RearwaveformSOAE.mat</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1518.0908203125</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.3832107514686146</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.001077367409704351</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.039696095494624</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.002190705121528471</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.0001954976909446787</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>TH13RearwaveformSOAE.mat</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2040.27099609375</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.2692127130766679</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.001237618494201748</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.9620902186494883</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.003174786133403373</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.0004291937523511609</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Human</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>TH13RearwaveformSOAE.mat</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>2697.03369140625</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E45" t="n">
         <v>0.08326029484050256</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F45" t="n">
         <v>0.001109814641365191</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G45" t="n">
         <v>0.4409908213593057</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H45" t="n">
         <v>0.003671008443831235</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I45" t="n">
         <v>3.926403002096487e-05</v>
       </c>
     </row>

</xml_diff>